<commit_message>
Finish add customer step
</commit_message>
<xml_diff>
--- a/ScenarioTesting/src/main/resources/dataset.xlsx
+++ b/ScenarioTesting/src/main/resources/dataset.xlsx
@@ -9,8 +9,10 @@
   </bookViews>
   <sheets>
     <sheet name="addLeaveTypeTest" sheetId="1" state="visible" r:id="rId2"/>
-    <sheet name="employee" sheetId="2" state="visible" r:id="rId3"/>
-    <sheet name="addSkillTest" sheetId="3" state="visible" r:id="rId4"/>
+    <sheet name="customer" sheetId="2" state="visible" r:id="rId3"/>
+    <sheet name="assignProjectTest" sheetId="3" state="visible" r:id="rId4"/>
+    <sheet name="employee" sheetId="4" state="visible" r:id="rId5"/>
+    <sheet name="addSkillTest" sheetId="5" state="visible" r:id="rId6"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -22,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="86">
   <si>
     <t xml:space="preserve">Testcase ID</t>
   </si>
@@ -118,6 +120,30 @@
   <si>
     <t xml:space="preserve">Error path: Insert an leave name with too long name
 - “Should not exceed 50 characters” error text pop out</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Index in testcase</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Description</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ASSIGN_PROJECT_TC000</t>
+  </si>
+  <si>
+    <t xml:space="preserve">John</t>
+  </si>
+  <si>
+    <t xml:space="preserve">test</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Jame</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Testcase Id</t>
   </si>
   <si>
     <t xml:space="preserve">Index</t>
@@ -640,9 +666,116 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
+  <dimension ref="A1:D3"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A6" activeCellId="0" sqref="A6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="28.76"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="15.46"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="D1" s="0" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="B2" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="C2" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="D2" s="0" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="B3" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C3" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="D3" s="0" t="s">
+        <v>32</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:A2"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="27.65"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="0" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
+        <v>30</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
   <dimension ref="A1:I3"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="J3" activeCellId="0" sqref="J3"/>
     </sheetView>
   </sheetViews>
@@ -658,31 +791,31 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>27</v>
+        <v>35</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>28</v>
+        <v>36</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>29</v>
+        <v>37</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>30</v>
+        <v>38</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>31</v>
+        <v>39</v>
       </c>
       <c r="F1" s="0" t="s">
-        <v>32</v>
+        <v>40</v>
       </c>
       <c r="G1" s="0" t="s">
-        <v>33</v>
+        <v>41</v>
       </c>
       <c r="H1" s="0" t="s">
-        <v>34</v>
+        <v>42</v>
       </c>
       <c r="I1" s="0" t="s">
-        <v>35</v>
+        <v>43</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -690,25 +823,25 @@
         <v>0</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>36</v>
+        <v>44</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>37</v>
+        <v>45</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>38</v>
+        <v>46</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>39</v>
+        <v>47</v>
       </c>
       <c r="F2" s="0" t="s">
-        <v>40</v>
+        <v>48</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>41</v>
+        <v>49</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>41</v>
+        <v>49</v>
       </c>
       <c r="I2" s="0" t="n">
         <v>1</v>
@@ -719,25 +852,25 @@
         <v>1</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>42</v>
+        <v>50</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>43</v>
+        <v>51</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>44</v>
+        <v>52</v>
       </c>
       <c r="E3" s="0" t="s">
-        <v>45</v>
+        <v>53</v>
       </c>
       <c r="F3" s="0" t="s">
-        <v>46</v>
+        <v>54</v>
       </c>
       <c r="G3" s="0" t="s">
-        <v>47</v>
+        <v>55</v>
       </c>
       <c r="H3" s="0" t="s">
-        <v>47</v>
+        <v>55</v>
       </c>
       <c r="I3" s="0" t="n">
         <v>0</v>
@@ -758,7 +891,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
@@ -783,10 +916,10 @@
         <v>0</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>48</v>
+        <v>56</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>49</v>
+        <v>57</v>
       </c>
       <c r="D1" s="0" t="s">
         <v>3</v>
@@ -797,168 +930,168 @@
     </row>
     <row r="2" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>50</v>
+        <v>58</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>51</v>
+        <v>59</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>52</v>
+        <v>60</v>
       </c>
       <c r="D2" s="0" t="n">
         <v>0</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>53</v>
+        <v>61</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>54</v>
+        <v>62</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>55</v>
+        <v>63</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>56</v>
+        <v>64</v>
       </c>
       <c r="D3" s="0" t="n">
         <v>0</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>53</v>
+        <v>61</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>57</v>
+        <v>65</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>58</v>
+        <v>66</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>59</v>
+        <v>67</v>
       </c>
       <c r="D4" s="0" t="n">
         <v>0</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>53</v>
+        <v>61</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>60</v>
+        <v>68</v>
       </c>
       <c r="B5" s="0" t="s">
+        <v>69</v>
+      </c>
+      <c r="C5" s="0" t="s">
+        <v>70</v>
+      </c>
+      <c r="D5" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E5" s="1" t="s">
         <v>61</v>
-      </c>
-      <c r="C5" s="0" t="s">
-        <v>62</v>
-      </c>
-      <c r="D5" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>53</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>63</v>
+        <v>71</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>51</v>
+        <v>59</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>52</v>
+        <v>60</v>
       </c>
       <c r="D6" s="0" t="n">
         <v>1</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>64</v>
+        <v>72</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>65</v>
+        <v>73</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>55</v>
+        <v>63</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>56</v>
+        <v>64</v>
       </c>
       <c r="D7" s="0" t="n">
         <v>1</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>64</v>
+        <v>72</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
+        <v>74</v>
+      </c>
+      <c r="B8" s="0" t="s">
         <v>66</v>
       </c>
-      <c r="B8" s="0" t="s">
-        <v>58</v>
-      </c>
       <c r="C8" s="0" t="s">
-        <v>59</v>
+        <v>67</v>
       </c>
       <c r="D8" s="0" t="n">
         <v>1</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>64</v>
+        <v>72</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>67</v>
+        <v>75</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>61</v>
+        <v>69</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>62</v>
+        <v>70</v>
       </c>
       <c r="D9" s="0" t="n">
         <v>1</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>64</v>
+        <v>72</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>68</v>
+        <v>76</v>
       </c>
       <c r="D10" s="0" t="n">
         <v>2</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>69</v>
+        <v>77</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
+        <v>78</v>
+      </c>
+      <c r="C11" s="0" t="s">
         <v>70</v>
-      </c>
-      <c r="C11" s="0" t="s">
-        <v>62</v>
       </c>
       <c r="D11" s="0" t="n">
         <v>2</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>69</v>
+        <v>77</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="124.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>71</v>
+        <v>79</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>25</v>
@@ -967,12 +1100,12 @@
         <v>3</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>72</v>
+        <v>80</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="124.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>73</v>
+        <v>81</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>25</v>
@@ -984,12 +1117,12 @@
         <v>4</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>74</v>
+        <v>82</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="124.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>75</v>
+        <v>83</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>25</v>
@@ -998,19 +1131,19 @@
         <v>5</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>76</v>
+        <v>84</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>77</v>
+        <v>85</v>
       </c>
       <c r="C15" s="1"/>
       <c r="D15" s="0" t="n">
         <v>2</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>69</v>
+        <v>77</v>
       </c>
     </row>
   </sheetData>

</xml_diff>